<commit_message>
Ajuste en escaleta - Organización
Organización de solicitudes gráficas y ajuste en escaleta.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion10/ESCALETA_ MA_09_10_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion10/ESCALETA_ MA_09_10_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\---Adriana\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -584,9 +583,6 @@
     <t>Refuerza tu aprendizaje: Las medidas de segmentos de la circunferencia</t>
   </si>
   <si>
-    <t>Competencias: La circunferencia y sus elementos en Cabri</t>
-  </si>
-  <si>
     <t>Banco de actividades: La circunferencia y la relaciones entres sus elementos</t>
   </si>
   <si>
@@ -728,6 +724,9 @@
   </si>
   <si>
     <t>Interactivo mediante el cual se explica cómo calcular la longitud de segmentos tangentes y secantes a la circunferencia.</t>
+  </si>
+  <si>
+    <t>Competencias: La circunferencia y sus elementos en GeoGebra</t>
   </si>
 </sst>
 </file>
@@ -1178,6 +1177,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1230,18 +1241,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1550,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K11" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="57" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1581,94 +1580,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="71" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="75" t="s">
+      <c r="I1" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="J1" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="J1" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="59" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="77" t="s">
+      <c r="P1" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="R1" s="80" t="s">
+      <c r="R1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="S1" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="T1" s="79" t="s">
+      <c r="T1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="U1" s="60" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="61"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="62"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="31" t="s">
         <v>93</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="78"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="60"/>
     </row>
     <row r="3" spans="1:21" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
@@ -1678,10 +1677,10 @@
         <v>104</v>
       </c>
       <c r="C3" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>188</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="53"/>
@@ -1723,7 +1722,7 @@
         <v>115</v>
       </c>
       <c r="T3" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U3" s="42" t="s">
         <v>116</v>
@@ -1737,10 +1736,10 @@
         <v>104</v>
       </c>
       <c r="C4" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>188</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="45"/>
@@ -1767,7 +1766,7 @@
         <v>97</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P4" s="46" t="s">
         <v>102</v>
@@ -1796,10 +1795,10 @@
         <v>104</v>
       </c>
       <c r="C5" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>188</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>105</v>
@@ -1843,7 +1842,7 @@
         <v>119</v>
       </c>
       <c r="T5" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U5" s="42" t="s">
         <v>120</v>
@@ -1857,10 +1856,10 @@
         <v>104</v>
       </c>
       <c r="C6" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>188</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="45"/>
@@ -1874,7 +1873,7 @@
         <v>103</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K6" s="36" t="s">
         <v>103</v>
@@ -1916,10 +1915,10 @@
         <v>104</v>
       </c>
       <c r="C7" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>188</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>106</v>
@@ -1935,7 +1934,7 @@
         <v>103</v>
       </c>
       <c r="J7" s="56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K7" s="36" t="s">
         <v>103</v>
@@ -1977,10 +1976,10 @@
         <v>104</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="45"/>
@@ -1994,7 +1993,7 @@
         <v>102</v>
       </c>
       <c r="J8" s="56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K8" s="36" t="s">
         <v>103</v>
@@ -2022,7 +2021,7 @@
         <v>115</v>
       </c>
       <c r="T8" s="43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U8" s="42" t="s">
         <v>116</v>
@@ -2036,10 +2035,10 @@
         <v>104</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="45"/>
@@ -2066,7 +2065,7 @@
       </c>
       <c r="N9" s="38"/>
       <c r="O9" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>102</v>
@@ -2095,10 +2094,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="45"/>
@@ -2112,7 +2111,7 @@
         <v>103</v>
       </c>
       <c r="J10" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>103</v>
@@ -2140,7 +2139,7 @@
         <v>119</v>
       </c>
       <c r="T10" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U10" s="42" t="s">
         <v>120</v>
@@ -2154,10 +2153,10 @@
         <v>104</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="45"/>
@@ -2171,7 +2170,7 @@
         <v>103</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K11" s="36" t="s">
         <v>103</v>
@@ -2184,7 +2183,7 @@
         <v>99</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>102</v>
@@ -2213,10 +2212,10 @@
         <v>104</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E12" s="50" t="s">
         <v>106</v>
@@ -2232,7 +2231,7 @@
         <v>103</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K12" s="36" t="s">
         <v>103</v>
@@ -2274,10 +2273,10 @@
         <v>104</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="45"/>
@@ -2319,7 +2318,7 @@
         <v>115</v>
       </c>
       <c r="T13" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U13" s="42" t="s">
         <v>116</v>
@@ -2333,7 +2332,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="57" t="s">
         <v>107</v>
@@ -2378,7 +2377,7 @@
         <v>119</v>
       </c>
       <c r="T14" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U14" s="42" t="s">
         <v>120</v>
@@ -2392,7 +2391,7 @@
         <v>104</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="57" t="s">
         <v>107</v>
@@ -2409,7 +2408,7 @@
         <v>103</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K15" s="36" t="s">
         <v>103</v>
@@ -2437,7 +2436,7 @@
         <v>119</v>
       </c>
       <c r="T15" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U15" s="42" t="s">
         <v>120</v>
@@ -2451,7 +2450,7 @@
         <v>104</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" s="57" t="s">
         <v>107</v>
@@ -2468,7 +2467,7 @@
         <v>103</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K16" s="36" t="s">
         <v>103</v>
@@ -2510,7 +2509,7 @@
         <v>104</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>107</v>
@@ -2529,7 +2528,7 @@
         <v>103</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>103</v>
@@ -2571,10 +2570,10 @@
         <v>104</v>
       </c>
       <c r="C18" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="45"/>
@@ -2630,10 +2629,10 @@
         <v>104</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="45"/>
@@ -2689,10 +2688,10 @@
         <v>104</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="45"/>
@@ -2734,7 +2733,7 @@
         <v>119</v>
       </c>
       <c r="T20" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U20" s="42" t="s">
         <v>120</v>
@@ -2748,10 +2747,10 @@
         <v>104</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E21" s="50" t="s">
         <v>106</v>
@@ -2795,7 +2794,7 @@
         <v>119</v>
       </c>
       <c r="T21" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U21" s="42" t="s">
         <v>120</v>
@@ -2809,10 +2808,10 @@
         <v>104</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="45"/>
@@ -2826,7 +2825,7 @@
         <v>102</v>
       </c>
       <c r="J22" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K22" s="36" t="s">
         <v>103</v>
@@ -2839,7 +2838,7 @@
       </c>
       <c r="N22" s="38"/>
       <c r="O22" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P22" s="46" t="s">
         <v>103</v>
@@ -2854,7 +2853,7 @@
         <v>115</v>
       </c>
       <c r="T22" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U22" s="47" t="s">
         <v>116</v>
@@ -2868,15 +2867,15 @@
         <v>104</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="45"/>
       <c r="G23" s="55" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H23" s="34">
         <v>21</v>
@@ -2885,7 +2884,7 @@
         <v>103</v>
       </c>
       <c r="J23" s="56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K23" s="36" t="s">
         <v>103</v>
@@ -2927,10 +2926,10 @@
         <v>104</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" s="50" t="s">
         <v>106</v>
@@ -2946,7 +2945,7 @@
         <v>103</v>
       </c>
       <c r="J24" s="56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K24" s="36" t="s">
         <v>103</v>
@@ -2959,7 +2958,7 @@
         <v>85</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>102</v>
@@ -2988,7 +2987,7 @@
         <v>104</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25" s="57" t="s">
         <v>109</v>
@@ -2998,7 +2997,7 @@
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="55" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="H25" s="34">
         <v>23</v>
@@ -3007,7 +3006,7 @@
         <v>103</v>
       </c>
       <c r="J25" s="56" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K25" s="36" t="s">
         <v>103</v>
@@ -3049,7 +3048,7 @@
         <v>104</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="57" t="s">
         <v>110</v>
@@ -3066,7 +3065,7 @@
         <v>103</v>
       </c>
       <c r="J26" s="56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K26" s="36" t="s">
         <v>103</v>
@@ -3094,7 +3093,7 @@
         <v>104</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D27" s="57" t="s">
         <v>110</v>
@@ -3102,7 +3101,7 @@
       <c r="E27" s="50"/>
       <c r="F27" s="45"/>
       <c r="G27" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H27" s="34">
         <v>25</v>
@@ -3111,7 +3110,7 @@
         <v>103</v>
       </c>
       <c r="J27" s="56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K27" s="36" t="s">
         <v>103</v>
@@ -3139,7 +3138,7 @@
         <v>119</v>
       </c>
       <c r="T27" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U27" s="42" t="s">
         <v>120</v>
@@ -3153,7 +3152,7 @@
         <v>104</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" s="57" t="s">
         <v>110</v>
@@ -3161,7 +3160,7 @@
       <c r="E28" s="50"/>
       <c r="F28" s="45"/>
       <c r="G28" s="55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H28" s="44">
         <v>26</v>
@@ -3170,7 +3169,7 @@
         <v>103</v>
       </c>
       <c r="J28" s="56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K28" s="36" t="s">
         <v>103</v>
@@ -3206,12 +3205,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -3226,6 +3219,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3 P6:P7 P9 P11:P13 P15:P17 P19:P21 P23:P27">

</xml_diff>